<commit_message>
Commented out code that output PDF in .py files
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cathy Hsu\Light and Motion\data_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D96FDB-D6C9-45CC-B076-7077CA0C1F90}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6CA94A-48AF-4D41-9971-BA11073C8EAC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E72AF285-2932-4A33-BA96-70EF447B094A}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Format</t>
   </si>
@@ -103,10 +103,13 @@
     <t>Skip First Row</t>
   </si>
   <si>
-    <t>5:8</t>
-  </si>
-  <si>
-    <t>4:71</t>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>2:30</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -462,7 +465,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -516,11 +519,14 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
       <c r="E3" t="s">
         <v>22</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -598,10 +604,13 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B2">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>75</v>
+        <v>100</v>
+      </c>
+      <c r="N2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>